<commit_message>
self rep question changed
</commit_message>
<xml_diff>
--- a/self_report.xlsx
+++ b/self_report.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF34D451-7D3F-4C2B-A48D-3B0900557E64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A028666-DB19-4843-B00C-DB61EC60B308}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -70,9 +70,6 @@
     <t>odd</t>
   </si>
   <si>
-    <t>Millise tunde viimase ploki tulemus sinus tekitas?</t>
-  </si>
-  <si>
     <t>Kui oluline oli sinu jaoks saada selles katses häid tulemusi?</t>
   </si>
   <si>
@@ -110,6 +107,9 @@
   </si>
   <si>
     <t>Kui miski tundus sulle selle katse juures imelik, pane see palun siia kirja</t>
+  </si>
+  <si>
+    <t>Millise tunde viimane plokk sinus tekitas?</t>
   </si>
 </sst>
 </file>
@@ -433,7 +433,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -469,13 +469,13 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
         <v>15</v>
-      </c>
-      <c r="E2" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -484,7 +484,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
@@ -502,7 +502,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
         <v>10</v>
@@ -523,13 +523,13 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D5" t="s">
         <v>6</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -538,16 +538,16 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D6" t="s">
         <v>6</v>
       </c>
       <c r="E6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -556,16 +556,16 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D7" t="s">
         <v>6</v>
       </c>
       <c r="E7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -574,16 +574,16 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D8" t="s">
         <v>6</v>
       </c>
       <c r="E8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -595,7 +595,7 @@
         <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>